<commit_message>
Add AGXL - IL, PIM - OR, CIM - MT,
</commit_message>
<xml_diff>
--- a/cypress/fixtures/expectedResults/Auto/PA IL 12 08 22.xlsx
+++ b/cypress/fixtures/expectedResults/Auto/PA IL 12 08 22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreis/MyOwnProject/api-test-cypress/cypress/fixtures/expectedResults/Auto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C702ED16-AA57-E742-B81E-C2D8F367F066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E29E578-7B9D-CC49-867D-D353A5FBBAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="-28300" windowWidth="33220" windowHeight="20040" xr2:uid="{992EAC74-168D-4556-9021-6B1FC9608133}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="186">
   <si>
     <t>CRITERIA</t>
   </si>
@@ -708,9 +708,6 @@
   </si>
   <si>
     <t>FEL</t>
-  </si>
-  <si>
-    <t>BUL</t>
   </si>
   <si>
     <t xml:space="preserve">  IL PA DOWNLOAD REV 07 22</t>
@@ -1237,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6089C9B-6C1F-41AA-9E90-19600F8F153D}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2355,9 +2352,6 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="B72" t="s">
         <v>163</v>
       </c>
@@ -2369,9 +2363,6 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="B73" t="s">
         <v>164</v>
       </c>
@@ -2401,7 +2392,7 @@
         <v>183</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C75" t="s">
         <v>149</v>
@@ -2410,7 +2401,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C76" s="19" t="s">
         <v>176</v>

</xml_diff>